<commit_message>
Upload Students and Create Exam Completed
</commit_message>
<xml_diff>
--- a/backend/uploads/Applicants_With_Group_ID_Template.xlsx
+++ b/backend/uploads/Applicants_With_Group_ID_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izma\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KASHAF\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887EEEA3-E8AA-4E99-833B-BF2DA6E46841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8035C108-0BE5-424B-809A-DC99FDB271FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H2" sqref="H2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +511,7 @@
         <v>12</v>
       </c>
       <c r="H2">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -537,7 +537,7 @@
         <v>17</v>
       </c>
       <c r="H3">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -563,7 +563,7 @@
         <v>21</v>
       </c>
       <c r="H4">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add applicants in Exam
</commit_message>
<xml_diff>
--- a/backend/uploads/Applicants_With_Group_ID_Template.xlsx
+++ b/backend/uploads/Applicants_With_Group_ID_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KASHAF\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439CDD78-FA08-4969-B29F-86CA5D2DB9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7CB2DF-67C8-4EFF-B100-2AC74F4395BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Full_Name</t>
   </si>
@@ -46,43 +46,64 @@
     <t>group_id</t>
   </si>
   <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>2002-05-14</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Ahmedabad, Gujarat</t>
+  </si>
+  <si>
+    <t>9123456789</t>
+  </si>
+  <si>
+    <t>2001-09-22</t>
+  </si>
+  <si>
     <t>Female</t>
   </si>
   <si>
     <t>Vadodara, Gujarat</t>
   </si>
   <si>
-    <t>vasudha@gmail.com</t>
-  </si>
-  <si>
-    <t>Vasudha@123</t>
-  </si>
-  <si>
-    <t>Vasudha Deshpande</t>
-  </si>
-  <si>
-    <t>Mumbai, Maharashtra</t>
-  </si>
-  <si>
-    <t>Anjali Patel</t>
-  </si>
-  <si>
-    <t>anjali@gmail.com</t>
-  </si>
-  <si>
-    <t>Anjali@123</t>
-  </si>
-  <si>
-    <t>Zubeda Tambe</t>
-  </si>
-  <si>
-    <t>zubeda@gmail.com</t>
-  </si>
-  <si>
-    <t>Zubeda@123</t>
-  </si>
-  <si>
-    <t>Dongri, Maharashtra</t>
+    <t>9988776655</t>
+  </si>
+  <si>
+    <t>2003-01-10</t>
+  </si>
+  <si>
+    <t>Surat, Gujarat</t>
+  </si>
+  <si>
+    <t>Aamena</t>
+  </si>
+  <si>
+    <t>aamenas@gmail.com</t>
+  </si>
+  <si>
+    <t>Akram</t>
+  </si>
+  <si>
+    <t>akram@gmail.com</t>
+  </si>
+  <si>
+    <t>Nazrin</t>
+  </si>
+  <si>
+    <t>nazzz@gmail.com</t>
+  </si>
+  <si>
+    <t>aamena@123</t>
+  </si>
+  <si>
+    <t>Akram@123</t>
+  </si>
+  <si>
+    <t>Nazrin@123</t>
   </si>
 </sst>
 </file>
@@ -127,10 +148,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -437,15 +457,12 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -476,80 +493,80 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>9872243210</v>
-      </c>
-      <c r="E2" s="2">
-        <v>38716</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>9123477789</v>
-      </c>
-      <c r="E3" s="2">
-        <v>37154</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
       <c r="H3">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>9988446655</v>
-      </c>
-      <c r="E4" s="2">
-        <v>37836</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
       <c r="H4">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -557,9 +574,9 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{52AD4E44-8850-4A4D-9A6E-793C0D080566}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{182C11B9-103C-47B1-9645-9D357A9B0E08}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{A78601B0-D0AF-4B12-9475-D457C205D97C}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{E5983186-01CE-42E5-9B6C-78D800BC921A}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{945498F5-1A5C-4A4F-9A5E-7A4677C00228}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{863CA9E8-B8F8-47AA-A556-BFAA7A657371}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{F265D703-4919-4D23-8244-5131FC890915}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{E792A25E-4C94-402A-B642-989E5704A05D}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{D196A949-80DB-4A4F-B437-8266F7110100}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>